<commit_message>
Login and Extracting W15 items
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A241907\Documents\UiPath\Client Hash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967B7143-E554-4E57-851F-FDF58244864F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061BE56B-0AD9-4154-BE0A-BEBB9D36D5FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -541,7 +541,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Update Work Item Component
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A241907\Documents\UiPath\Client Hash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061BE56B-0AD9-4154-BE0A-BEBB9D36D5FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AED6B36-FB51-47A5-A667-24737361F1CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -163,13 +163,19 @@
   </si>
   <si>
     <t>ACME_Credentials</t>
+  </si>
+  <si>
+    <t>EmailAcccount</t>
+  </si>
+  <si>
+    <t>kakoozaa2@stanbic.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -193,6 +199,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -211,10 +223,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -224,8 +237,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -541,7 +556,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -626,7 +641,14 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1620,8 +1642,11 @@
     <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{7476B353-7F12-4B3C-A639-38E8375C9010}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>